<commit_message>
Problems with big memory
</commit_message>
<xml_diff>
--- a/BIOQ245.xlsx
+++ b/BIOQ245.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -102,112 +102,196 @@
     <t>Results.xlsx</t>
   </si>
   <si>
-    <t>Rules - 1</t>
+    <t>Rules - Age</t>
   </si>
   <si>
     <t>value &lt; 20</t>
   </si>
   <si>
+    <t>Teenage</t>
+  </si>
+  <si>
     <t>value &gt;= 20 &amp;&amp; value &lt; 30</t>
   </si>
   <si>
+    <t>20s</t>
+  </si>
+  <si>
     <t>value &gt;= 30 &amp;&amp; value &lt; 40</t>
   </si>
   <si>
+    <t>30s</t>
+  </si>
+  <si>
     <t>value &gt;= 40</t>
   </si>
   <si>
-    <t>Rules - 6</t>
+    <t>old</t>
+  </si>
+  <si>
+    <t>Rules - Sex</t>
   </si>
   <si>
     <t>value == 1</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
     <t>value == 2</t>
   </si>
   <si>
-    <t>Rules - 9</t>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Rules - BMI</t>
   </si>
   <si>
     <t>value &lt;= 18.5</t>
   </si>
   <si>
+    <t>Underweight</t>
+  </si>
+  <si>
     <t>value &gt; 18.5 &amp;&amp; value &lt; 25</t>
   </si>
   <si>
+    <t>Healthy</t>
+  </si>
+  <si>
     <t>value &gt;= 25 &amp;&amp; value &lt; 30</t>
   </si>
   <si>
+    <t>Overweight</t>
+  </si>
+  <si>
     <t>value &gt;= 30</t>
   </si>
   <si>
-    <t>Rules - 14</t>
+    <t>Obese</t>
+  </si>
+  <si>
+    <t>Rules - Marital</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>Married</t>
   </si>
   <si>
     <t>value == 3</t>
   </si>
   <si>
-    <t>Rules - 18</t>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Rules - Children</t>
   </si>
   <si>
     <t>value == 0</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>value &gt; 0</t>
   </si>
   <si>
-    <t>Rules - 21</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Rules - Sleep</t>
   </si>
   <si>
     <t>value &lt; 7</t>
   </si>
   <si>
+    <t>Poor</t>
+  </si>
+  <si>
     <t>value &gt;= 7</t>
   </si>
   <si>
-    <t>Rules - 24</t>
-  </si>
-  <si>
-    <t>Rules - 27</t>
+    <t>Enough</t>
+  </si>
+  <si>
+    <t>Rules - Pt_ft</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Rules - Cigs</t>
   </si>
   <si>
     <t>value &lt;= 1</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>value &gt; 1</t>
   </si>
   <si>
-    <t>Rules - 30</t>
-  </si>
-  <si>
-    <t>Rules - 33</t>
-  </si>
-  <si>
-    <t>Rules - 37</t>
-  </si>
-  <si>
-    <t>Rules - 46</t>
+    <t>Rules - Chol</t>
+  </si>
+  <si>
+    <t>Rules - Fruit</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>Rules - Veg</t>
+  </si>
+  <si>
+    <t>Rules - Walk_times</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>value &lt;= 7</t>
+  </si>
+  <si>
+    <t>Commuter</t>
+  </si>
+  <si>
+    <t>value &gt; 7 &amp;&amp; value &lt;= 14</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>value &gt; 14</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Rules - Walk_mins</t>
   </si>
   <si>
     <t>value &lt;= 70</t>
   </si>
   <si>
+    <t>CouchPotato</t>
+  </si>
+  <si>
     <t>value &gt; 70 &amp;&amp; value &lt;= 140</t>
   </si>
   <si>
+    <t>Regular</t>
+  </si>
+  <si>
     <t>value &gt; 140</t>
-  </si>
-  <si>
-    <t>Rules - 41</t>
-  </si>
-  <si>
-    <t>value &lt;= 7</t>
-  </si>
-  <si>
-    <t>value &gt; 7 &amp;&amp; value &lt;= 14</t>
-  </si>
-  <si>
-    <t>value &gt; 14</t>
   </si>
 </sst>
 </file>
@@ -221,31 +305,31 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="8"/>
       <name val="Courier New"/>
+      <family val="3"/>
       <charset val="1"/>
-      <family val="3"/>
-      <sz val="8"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Courier New"/>
+      <family val="3"/>
       <charset val="1"/>
-      <family val="3"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,21 +428,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.0414201183432"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="5.18934911242604"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62130177514793"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.905325443787"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.62130177514793"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.47337278106509"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.0532544378698"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.75739644970414"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.905325443787"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="7.47337278106509"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="6.32544378698225"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.47337278106509"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="5.18934911242604"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.2011834319527"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.0532544378698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.0414201183432"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="5.18934911242604"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62130177514793"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.905325443787"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.62130177514793"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.47337278106509"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.0532544378698"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.75739644970414"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.905325443787"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.47337278106509"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.32544378698225"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.47337278106509"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="5.18934911242604"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.2011834319527"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.0532544378698"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="13.3609467455621"/>
   </cols>
   <sheetData>
@@ -5674,13 +5758,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D59"/>
+  <dimension ref="B2:D65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A27" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="G53" activeCellId="0" pane="topLeft" sqref="G53"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A49" activeCellId="0" pane="topLeft" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="9.7"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85207100591716"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7869822485207"/>
@@ -5688,7 +5772,6 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.85207100591716"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="1"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="2">
       <c r="B2" s="6" t="s">
         <v>18</v>
@@ -5761,353 +5844,353 @@
       <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6" t="n">
-        <v>2</v>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="12">
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="13">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="15">
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="16">
       <c r="C16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>7</v>
+        <v>37</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="17">
       <c r="C17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="6" t="n">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="19">
       <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="20">
       <c r="C20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="6" t="n">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="21">
       <c r="C21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="6" t="n">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="22">
       <c r="C22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>13</v>
+        <v>48</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="23">
       <c r="B23" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>16</v>
+        <v>39</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="26">
       <c r="C26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="27">
       <c r="B27" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>23</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="33">
       <c r="B33" s="0" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="36">
+        <v>39</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.85" outlineLevel="0" r="36">
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>28</v>
+        <v>69</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="39">
+        <v>71</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.85" outlineLevel="0" r="39">
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="42">
       <c r="B42" s="0" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="44">
       <c r="C44" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>36</v>
+        <v>71</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="46">
       <c r="B46" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="50">
-      <c r="B50" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="51">
-      <c r="C51" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="60">
+      <c r="B60" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="61">
+      <c r="C61" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="0" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="52">
-      <c r="C52" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="53">
-      <c r="C53" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="54"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="55">
-      <c r="B55" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="56">
-      <c r="C56" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="57">
-      <c r="C57" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="58">
-      <c r="C58" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="59">
-      <c r="C59" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="0" t="n">
-        <v>45</v>
-      </c>
-    </row>
+      <c r="D61" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="62">
+      <c r="C62" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="63">
+      <c r="C63" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="64">
+      <c r="C64" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.85" outlineLevel="0" r="65">
+      <c r="B65" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.85" outlineLevel="0" r="66">
+      <c r="C66" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="67">
+      <c r="C67" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="9.7" outlineLevel="0" r="68">
+      <c r="C68" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Some parallelism and attempt to use Jruby
</commit_message>
<xml_diff>
--- a/BIOQ245.xlsx
+++ b/BIOQ245.xlsx
@@ -305,31 +305,31 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <name val="Courier New"/>
+      <charset val="1"/>
+      <family val="3"/>
       <sz val="8"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Courier New"/>
+      <charset val="1"/>
+      <family val="3"/>
       <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5760,8 +5760,8 @@
   </sheetPr>
   <dimension ref="B2:D65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="A49" activeCellId="0" pane="topLeft" sqref="A49"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A30" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A64" activeCellId="0" pane="topLeft" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="9.7"/>

</xml_diff>